<commit_message>
Merge in missing sales tax data
</commit_message>
<xml_diff>
--- a/Shocks/SalesTax/MissingData/MissingData.xlsx
+++ b/Shocks/SalesTax/MissingData/MissingData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliciazhang/Documents/GitHub/Wage-Price-Rigidity/Shocks/SalesTax/MissingData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4AD73E-9268-8541-A601-289AFBA54DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E950C9B7-47B2-DA4A-B7DE-76DD8E2F3FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7820" yWindow="760" windowWidth="19080" windowHeight="16160" xr2:uid="{372949AB-D1E5-6F40-BDA0-2A804D144C58}"/>
+    <workbookView xWindow="9600" yWindow="520" windowWidth="19080" windowHeight="16160" xr2:uid="{372949AB-D1E5-6F40-BDA0-2A804D144C58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552281E1-C520-8744-AF31-224E842B3E41}">
   <dimension ref="A1:F205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A155" sqref="A155:XFD155"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="F207" sqref="F207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3293,6 +3293,9 @@
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="6"/>
+      <c r="F156">
+        <v>2009</v>
+      </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
@@ -3303,6 +3306,9 @@
       </c>
       <c r="C157" s="5"/>
       <c r="D157" s="6"/>
+      <c r="F157">
+        <v>2009</v>
+      </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
@@ -3313,6 +3319,9 @@
       </c>
       <c r="C158" s="5"/>
       <c r="D158" s="6"/>
+      <c r="F158">
+        <v>2009</v>
+      </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
@@ -3323,6 +3332,9 @@
       </c>
       <c r="C159" s="5"/>
       <c r="D159" s="6"/>
+      <c r="F159">
+        <v>2009</v>
+      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
@@ -3333,8 +3345,11 @@
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F160">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>18</v>
       </c>
@@ -3342,8 +3357,11 @@
         <v>6</v>
       </c>
       <c r="D161" s="6"/>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F161">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>19</v>
       </c>
@@ -3351,8 +3369,11 @@
         <v>7</v>
       </c>
       <c r="D162" s="6"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F162">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>20</v>
       </c>
@@ -3361,8 +3382,11 @@
       </c>
       <c r="C163" s="5"/>
       <c r="D163" s="6"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F163">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>21</v>
       </c>
@@ -3371,8 +3395,11 @@
       </c>
       <c r="C164" s="5"/>
       <c r="D164" s="6"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F164">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>22</v>
       </c>
@@ -3381,8 +3408,11 @@
       </c>
       <c r="C165" s="5"/>
       <c r="D165" s="6"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F165">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>23</v>
       </c>
@@ -3390,8 +3420,11 @@
         <v>6</v>
       </c>
       <c r="D166" s="6"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F166">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>60</v>
       </c>
@@ -3400,8 +3433,11 @@
       </c>
       <c r="C167" s="5"/>
       <c r="D167" s="6"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F167">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>24</v>
       </c>
@@ -3409,8 +3445,11 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="D168" s="6"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F168">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>25</v>
       </c>
@@ -3419,8 +3458,11 @@
       </c>
       <c r="C169" s="5"/>
       <c r="D169" s="6"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F169">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>26</v>
       </c>
@@ -3429,8 +3471,11 @@
       </c>
       <c r="C170" s="5"/>
       <c r="D170" s="6"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F170">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>27</v>
       </c>
@@ -3438,8 +3483,11 @@
         <v>6</v>
       </c>
       <c r="D171" s="6"/>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F171">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>28</v>
       </c>
@@ -3448,8 +3496,11 @@
       </c>
       <c r="C172" s="5"/>
       <c r="D172" s="6"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F172">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>29</v>
       </c>
@@ -3457,8 +3508,11 @@
         <v>5</v>
       </c>
       <c r="D173" s="6"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F173">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>30</v>
       </c>
@@ -3466,8 +3520,11 @@
         <v>6</v>
       </c>
       <c r="D174" s="6"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F174">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>31</v>
       </c>
@@ -3475,8 +3532,11 @@
         <v>6.25</v>
       </c>
       <c r="D175" s="6"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F175">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>32</v>
       </c>
@@ -3484,8 +3544,11 @@
         <v>6</v>
       </c>
       <c r="D176" s="6"/>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F176">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>33</v>
       </c>
@@ -3494,8 +3557,11 @@
       </c>
       <c r="C177" s="5"/>
       <c r="D177" s="6"/>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F177">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>34</v>
       </c>
@@ -3503,8 +3569,11 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="D178" s="6"/>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F178">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>35</v>
       </c>
@@ -3513,8 +3582,11 @@
       </c>
       <c r="C179" s="5"/>
       <c r="D179" s="6"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F179">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>36</v>
       </c>
@@ -3522,8 +3594,11 @@
         <v>7</v>
       </c>
       <c r="D180" s="6"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F180">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>37</v>
       </c>
@@ -3532,8 +3607,11 @@
       </c>
       <c r="C181" s="5"/>
       <c r="D181" s="6"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F181">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>38</v>
       </c>
@@ -3542,8 +3620,11 @@
       </c>
       <c r="C182" s="5"/>
       <c r="D182" s="6"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F182">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>39</v>
       </c>
@@ -3551,8 +3632,11 @@
         <v>7</v>
       </c>
       <c r="D183" s="6"/>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F183">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>40</v>
       </c>
@@ -3560,8 +3644,11 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="D184" s="6"/>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F184">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>41</v>
       </c>
@@ -3570,8 +3657,11 @@
       </c>
       <c r="C185" s="5"/>
       <c r="D185" s="6"/>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F185">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>42</v>
       </c>
@@ -3580,8 +3670,11 @@
       </c>
       <c r="C186" s="5"/>
       <c r="D186" s="6"/>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F186">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>43</v>
       </c>
@@ -3590,8 +3683,11 @@
       </c>
       <c r="C187" s="5"/>
       <c r="D187" s="6"/>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F187">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>44</v>
       </c>
@@ -3600,8 +3696,11 @@
       </c>
       <c r="C188" s="5"/>
       <c r="D188" s="6"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F188">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>45</v>
       </c>
@@ -3610,8 +3709,11 @@
       </c>
       <c r="C189" s="5"/>
       <c r="D189" s="6"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F189">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>46</v>
       </c>
@@ -3620,8 +3722,11 @@
       </c>
       <c r="C190" s="5"/>
       <c r="D190" s="6"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F190">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>47</v>
       </c>
@@ -3629,8 +3734,11 @@
         <v>7</v>
       </c>
       <c r="D191" s="6"/>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F191">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>48</v>
       </c>
@@ -3639,8 +3747,11 @@
       </c>
       <c r="C192" s="5"/>
       <c r="D192" s="6"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F192">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>49</v>
       </c>
@@ -3648,8 +3759,11 @@
         <v>7.0000000000000009</v>
       </c>
       <c r="D193" s="6"/>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F193">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>50</v>
       </c>
@@ -3658,8 +3772,11 @@
       </c>
       <c r="C194" s="5"/>
       <c r="D194" s="6"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F194">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>51</v>
       </c>
@@ -3668,8 +3785,11 @@
       </c>
       <c r="C195" s="5"/>
       <c r="D195" s="6"/>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F195">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>52</v>
       </c>
@@ -3678,8 +3798,11 @@
       </c>
       <c r="C196" s="5"/>
       <c r="D196" s="6"/>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F196">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>53</v>
       </c>
@@ -3688,8 +3811,11 @@
       </c>
       <c r="C197" s="5"/>
       <c r="D197" s="6"/>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F197">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>54</v>
       </c>
@@ -3698,8 +3824,11 @@
       </c>
       <c r="C198" s="5"/>
       <c r="D198" s="6"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F198">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>55</v>
       </c>
@@ -3707,8 +3836,11 @@
         <v>6</v>
       </c>
       <c r="D199" s="6"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F199">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>56</v>
       </c>
@@ -3716,8 +3848,11 @@
         <v>5</v>
       </c>
       <c r="D200" s="6"/>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F200">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>57</v>
       </c>
@@ -3726,8 +3861,11 @@
       </c>
       <c r="C201" s="5"/>
       <c r="D201" s="6"/>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F201">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>58</v>
       </c>
@@ -3735,8 +3873,11 @@
         <v>6</v>
       </c>
       <c r="D202" s="6"/>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F202">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>59</v>
       </c>
@@ -3745,8 +3886,11 @@
       </c>
       <c r="C203" s="5"/>
       <c r="D203" s="6"/>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F203">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>61</v>
       </c>
@@ -3755,8 +3899,11 @@
       </c>
       <c r="C204" s="5"/>
       <c r="D204" s="6"/>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F204">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>70</v>
       </c>
@@ -3764,6 +3911,9 @@
         <v>6</v>
       </c>
       <c r="D205" s="6"/>
+      <c r="F205">
+        <v>2009</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>